<commit_message>
change in testdata and test methods
</commit_message>
<xml_diff>
--- a/Resources/TestData/ControlFile.xlsx
+++ b/Resources/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="5130" tabRatio="919"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="5130" tabRatio="919" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="14" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>Password</t>
   </si>
@@ -236,6 +236,15 @@
   </si>
   <si>
     <t>عبدالغني السيد</t>
+  </si>
+  <si>
+    <t>demo1@demo.com</t>
+  </si>
+  <si>
+    <t>demo2</t>
+  </si>
+  <si>
+    <t>demo2@demo.com</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1090,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1480,8 +1489,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,8 +1515,8 @@
       <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>60</v>
+      <c r="B2" s="34" t="s">
+        <v>70</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>60</v>
@@ -1517,11 +1526,11 @@
       <c r="A3" s="32">
         <v>2</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>60</v>
+      <c r="B3" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>